<commit_message>
Updated TCSs for QARSF as per Read Excel Path changes
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/CustomerMaster.xlsx
+++ b/templates/AutomationOrg/CustomerMaster.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_AutomationOrg\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CACC0D9-CB05-47C5-BA36-32036A630AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85390D5D-B866-4620-9108-6FFBF80FEE6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22590" yWindow="2340" windowWidth="23415" windowHeight="7875" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddHeader_Invoicing&amp;Credit" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="30">
   <si>
     <t>API Mode</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>a6B5f000000PqAT</t>
+  </si>
+  <si>
+    <t>AUTOMATIONCUST-3</t>
   </si>
 </sst>
 </file>
@@ -814,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D2E608B-C35A-4DF1-88E4-ACEE9E872FF5}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,7 +888,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -897,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFB83414-1FDB-48B7-AD90-293B7141913A}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>